<commit_message>
Just. One. More. Change.
The excel spreadsheet is troublesome - some of the insert statements are
no longer accurate and require troubleshooting on the fly.
</commit_message>
<xml_diff>
--- a/rs tablespace definition.xlsx
+++ b/rs tablespace definition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="810" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="810" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ts_radiosilence" sheetId="19" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="152">
   <si>
     <t>History</t>
   </si>
@@ -475,6 +475,21 @@
   </si>
   <si>
     <t>Unreal Object</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
@@ -859,7 +874,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1144,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,9 +1237,52 @@
       <c r="A2" t="s">
         <v>125</v>
       </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
       <c r="C2" s="3" t="str">
         <f>$C$1 &amp; "'" &amp; A2 &amp; "', '" &amp; B2 &amp; "');"</f>
-        <v>INSERT INTO rs_contact_subject (contact_Id, subject_Id) values ('RS0', '');</v>
+        <v>INSERT INTO rs_contact_subject (contact_Id, subject_Id) values ('RS0', 'S0');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1836,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2211,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,8 +2938,8 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="str">
-        <f>"INSERT INTO subjects (" &amp; A1 &amp; ", " &amp;  B1 &amp; ") values ("</f>
-        <v>INSERT INTO subjects (subject_Id, subject) values (</v>
+        <f>"INSERT INTO subjectList (" &amp; A1 &amp; ", " &amp;  B1 &amp; ") values ("</f>
+        <v>INSERT INTO subjectList (subject_Id, subject) values (</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>27</v>
@@ -2912,7 +2970,7 @@
       </c>
       <c r="C2" s="3" t="str">
         <f>C$1 &amp; "'" &amp; A2 &amp; "',  '" &amp; B2 &amp; "' );"</f>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S0',  'Math' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S0',  'Math' );</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -2931,7 +2989,7 @@
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" ref="C3:C29" si="1">C$1 &amp; "'" &amp; A3 &amp; "',  '" &amp; B3 &amp; "' );"</f>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S1',  'English' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S1',  'English' );</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -2950,7 +3008,7 @@
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S2',  'Proofreading' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S2',  'Proofreading' );</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -2972,7 +3030,7 @@
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S3',  'Accounting' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S3',  'Accounting' );</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
@@ -2991,7 +3049,7 @@
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S4',  'Computer Science' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S4',  'Computer Science' );</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -3022,7 +3080,7 @@
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S5',  'Electrical Engineering' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S5',  'Electrical Engineering' );</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3035,7 +3093,7 @@
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S6',  'History' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S6',  'History' );</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3048,7 +3106,7 @@
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S7',  'Blackboard' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S7',  'Blackboard' );</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3061,7 +3119,7 @@
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S8',  'General Computer Help' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S8',  'General Computer Help' );</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3074,7 +3132,7 @@
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S9',  'Microsoft Applications' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S9',  'Microsoft Applications' );</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3087,7 +3145,7 @@
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S10',  'Business Management' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S10',  'Business Management' );</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3100,7 +3158,7 @@
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S11',  'Microbiology' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S11',  'Microbiology' );</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3113,7 +3171,7 @@
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S12',  'Critical Thinking' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S12',  'Critical Thinking' );</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3126,7 +3184,7 @@
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S13',  'Engineering' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S13',  'Engineering' );</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3139,7 +3197,7 @@
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S14',  'Psychology' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S14',  'Psychology' );</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3152,7 +3210,7 @@
       </c>
       <c r="C17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S15',  'Economics' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S15',  'Economics' );</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3165,7 +3223,7 @@
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S16',  'Chemistry' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S16',  'Chemistry' );</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3178,7 +3236,7 @@
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S17',  'Earth Science' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S17',  'Earth Science' );</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3191,7 +3249,7 @@
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S18',  'CADD' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S18',  'CADD' );</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3204,7 +3262,7 @@
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S19',  'Early Childhood Education' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S19',  'Early Childhood Education' );</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3217,7 +3275,7 @@
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S20',  'Sociology' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S20',  'Sociology' );</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3230,7 +3288,7 @@
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S21',  'A and P' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S21',  'A and P' );</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,7 +3301,7 @@
       </c>
       <c r="C24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S22',  'Medical Terminology' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S22',  'Medical Terminology' );</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3256,7 +3314,7 @@
       </c>
       <c r="C25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S23',  'Marketing' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S23',  'Marketing' );</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3269,7 +3327,7 @@
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S24',  'Biology' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S24',  'Biology' );</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3282,7 +3340,7 @@
       </c>
       <c r="C27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S25',  'Physics' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S25',  'Physics' );</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3295,7 +3353,7 @@
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S26',  'APA' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S26',  'APA' );</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,7 +3366,7 @@
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO subjects (subject_Id, subject) values ('S27',  'MLA' );</v>
+        <v>INSERT INTO subjectList (subject_Id, subject) values ('S27',  'MLA' );</v>
       </c>
     </row>
   </sheetData>

</xml_diff>